<commit_message>
adding a small comparison for europe
</commit_message>
<xml_diff>
--- a/ressources/index_codes.xlsx
+++ b/ressources/index_codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinSchmitz\CODING\factornessy\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2ACF6E-110F-4C94-8BC3-A492799EBB8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3744AF63-69FD-4207-87A2-E01FDB56134D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{894CFF15-4DEC-410B-8396-437E0DDF0909}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>name</t>
   </si>
@@ -124,13 +124,43 @@
   </si>
   <si>
     <t>iShares</t>
+  </si>
+  <si>
+    <t>costs</t>
+  </si>
+  <si>
+    <t>LU0486851024</t>
+  </si>
+  <si>
+    <t>Value (Europe)</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Momentum (Europe)</t>
+  </si>
+  <si>
+    <t>IE00BQN1K786</t>
+  </si>
+  <si>
+    <t>Small-Cap (Value) (Europe)</t>
+  </si>
+  <si>
+    <t>IE00BSPLC298</t>
+  </si>
+  <si>
+    <t>MSCI World (Europe)</t>
+  </si>
+  <si>
+    <t>LU0274209237</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,16 +168,328 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -155,15 +497,220 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="50">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="46" xr:uid="{8D071BE7-0F26-46A3-871F-86D3836638E9}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 16" xfId="42" xr:uid="{08037F39-D1B4-40A8-8274-D102E0A0847D}"/>
+    <cellStyle name="Normal 2" xfId="43" xr:uid="{0D436DCA-1D4D-4FDB-BE71-5E34451A5FB9}"/>
+    <cellStyle name="Normal 3" xfId="44" xr:uid="{A9AA141C-9691-4B91-9E67-A42F3C3D1D0F}"/>
+    <cellStyle name="Normal 3 2" xfId="47" xr:uid="{5FA26B13-A0D8-402E-A70B-5764F157792F}"/>
+    <cellStyle name="Normal 4" xfId="45" xr:uid="{259820A6-4687-4F5F-905A-A0F8ADEA221B}"/>
+    <cellStyle name="Normal 4 2" xfId="48" xr:uid="{E8946A74-D28E-4CFD-BE9D-77D50E8DA97B}"/>
+    <cellStyle name="Normal 5" xfId="49" xr:uid="{851F0FEE-55D6-4E6C-9BA1-A28C788EF4C8}"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -475,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170B0C18-B286-482A-A5E0-3D1A59B9725A}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +1037,7 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,8 +1056,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -527,7 +1077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -544,7 +1094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -561,7 +1111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -578,7 +1128,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -595,7 +1145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -612,7 +1162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -629,7 +1179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -649,7 +1199,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -664,6 +1214,86 @@
       </c>
       <c r="E10" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>705382</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>701601</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>139245</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>990500</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding the asset allocations to the volatility charts
</commit_message>
<xml_diff>
--- a/ressources/index_codes.xlsx
+++ b/ressources/index_codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinSchmitz\CODING\factornessy\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3744AF63-69FD-4207-87A2-E01FDB56134D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F73485-FBB9-47A9-BBB2-3D89A2DE8729}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{894CFF15-4DEC-410B-8396-437E0DDF0909}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>name</t>
   </si>
@@ -154,6 +154,30 @@
   </si>
   <si>
     <t>LU0274209237</t>
+  </si>
+  <si>
+    <t>IE00BYYHSM20</t>
+  </si>
+  <si>
+    <t>High Dividend (Europe)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iShares </t>
+  </si>
+  <si>
+    <t>IE00BG0SKF03</t>
+  </si>
+  <si>
+    <t>Value (EM)</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>Momentum (EM)</t>
+  </si>
+  <si>
+    <t>Small-Cap (Value) (EM)</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170B0C18-B286-482A-A5E0-3D1A59B9725A}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,6 +1320,68 @@
         <v>0.12</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>713283</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>719637</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <v>703757</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>702239</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
just progress across the board
</commit_message>
<xml_diff>
--- a/ressources/index_codes.xlsx
+++ b/ressources/index_codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinSchmitz\CODING\factornessy\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F73485-FBB9-47A9-BBB2-3D89A2DE8729}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A9B01D-5884-46DA-A937-A30456EF771D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{894CFF15-4DEC-410B-8396-437E0DDF0909}"/>
   </bookViews>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
trying to add EM to the analysis, which does not work because its not daily.
</commit_message>
<xml_diff>
--- a/ressources/index_codes.xlsx
+++ b/ressources/index_codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinSchmitz\CODING\factornessy\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A9B01D-5884-46DA-A937-A30456EF771D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27565D9F-5429-4795-A54B-7E917BE43A81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{894CFF15-4DEC-410B-8396-437E0DDF0909}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>name</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Small-Cap (Value) (EM)</t>
+  </si>
+  <si>
+    <t>EM IMI (EM)</t>
+  </si>
+  <si>
+    <t>IE00BKM4GZ66</t>
+  </si>
+  <si>
+    <t>ishares</t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170B0C18-B286-482A-A5E0-3D1A59B9725A}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,7 +1369,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1371,7 +1380,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1380,6 +1389,26 @@
       </c>
       <c r="C18" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>664220</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19">
+        <v>0.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding a comparison to household names
</commit_message>
<xml_diff>
--- a/ressources/index_codes.xlsx
+++ b/ressources/index_codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinSchmitz\CODING\factornessy\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27565D9F-5429-4795-A54B-7E917BE43A81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4611E1A-4A06-420D-BF9C-E650ADC3A491}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{894CFF15-4DEC-410B-8396-437E0DDF0909}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>name</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>ishares</t>
+  </si>
+  <si>
+    <t>EM LibertyQ (EM)</t>
+  </si>
+  <si>
+    <t>LibertyQ</t>
   </si>
 </sst>
 </file>
@@ -1055,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170B0C18-B286-482A-A5E0-3D1A59B9725A}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,6 +1417,23 @@
         <v>0.18</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20">
+        <v>709646</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20">
+        <v>0.45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added one-time deposit analysis
</commit_message>
<xml_diff>
--- a/ressources/index_codes.xlsx
+++ b/ressources/index_codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinSchmitz\CODING\factornessy\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4611E1A-4A06-420D-BF9C-E650ADC3A491}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C74A7CC-7339-437B-9D7F-489A83672E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{894CFF15-4DEC-410B-8396-437E0DDF0909}"/>
+    <workbookView xWindow="26265" yWindow="900" windowWidth="28770" windowHeight="14700" xr2:uid="{894CFF15-4DEC-410B-8396-437E0DDF0909}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,10 +189,10 @@
     <t>ishares</t>
   </si>
   <si>
-    <t>EM LibertyQ (EM)</t>
-  </si>
-  <si>
     <t>LibertyQ</t>
+  </si>
+  <si>
+    <t>FLXE</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20">
         <v>709646</v>
@@ -1428,7 +1428,7 @@
         <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20">
         <v>0.45</v>

</xml_diff>